<commit_message>
Finished the logic to upload massive amount of data on to the database in seconds
</commit_message>
<xml_diff>
--- a/DBTester/wwwroot/UPC.xlsx
+++ b/DBTester/wwwroot/UPC.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7449FF41-8CEC-4D2A-8DB0-83892BE90D75}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E338772C-4140-4CC9-9B89-48152F5AF0C9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Price List Enhanced" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -866,11 +866,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,175 +888,178 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>539808</v>
+        <v>540320</v>
       </c>
       <c r="B2" s="1">
-        <v>737052581248</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>482296</v>
+        <v>539808</v>
       </c>
       <c r="B3" s="1">
-        <v>737052581309</v>
+        <v>737052581248</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>511013</v>
+        <v>482296</v>
       </c>
       <c r="B4" s="1">
-        <v>737052581330</v>
+        <v>737052581309</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>540250</v>
+        <v>511013</v>
       </c>
       <c r="B5" s="1">
-        <v>737052947792</v>
+        <v>737052581330</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>534811</v>
+        <v>540250</v>
       </c>
       <c r="B6" s="1">
-        <v>737052676838</v>
+        <v>737052947792</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>502284</v>
+        <v>534811</v>
       </c>
       <c r="B7" s="1">
-        <v>737052676869</v>
+        <v>737052676838</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>512069</v>
+        <v>502284</v>
       </c>
       <c r="B8" s="1">
-        <v>737052739373</v>
+        <v>737052676869</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>512067</v>
+        <v>512069</v>
       </c>
       <c r="B9" s="1">
-        <v>737052739410</v>
+        <v>737052739373</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>540856</v>
+        <v>512067</v>
       </c>
       <c r="B10" s="1">
-        <v>130601009765</v>
+        <v>737052739410</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>460836</v>
+        <v>540856</v>
       </c>
       <c r="B11" s="1">
-        <v>3349666007891</v>
+        <v>130601009765</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>460272</v>
+        <v>460836</v>
       </c>
       <c r="B12" s="1">
-        <v>3349666007914</v>
+        <v>3349666007891</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>453437</v>
+        <v>460272</v>
       </c>
       <c r="B13" s="1">
-        <v>3349666007921</v>
+        <v>3349666007914</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>466518</v>
+        <v>453437</v>
       </c>
       <c r="B14" s="1">
-        <v>3349666007945</v>
+        <v>3349666007921</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>490516</v>
+        <v>466518</v>
       </c>
       <c r="B15" s="1">
-        <v>3349666007983</v>
+        <v>3349666007945</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>489386</v>
+        <v>490516</v>
       </c>
       <c r="B16" s="1">
-        <v>3349668509669</v>
+        <v>3349666007983</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>538941</v>
+        <v>489386</v>
       </c>
       <c r="B17" s="1">
-        <v>3349668542826</v>
+        <v>3349668509669</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>538671</v>
+        <v>538941</v>
       </c>
       <c r="B18" s="1">
-        <v>3349668546282</v>
+        <v>3349668542826</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>524924</v>
+        <v>538671</v>
       </c>
       <c r="B19" s="1">
-        <v>3349668530045</v>
+        <v>3349668546282</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>539811</v>
+        <v>524924</v>
       </c>
       <c r="B20" s="1">
-        <v>3349668530069</v>
+        <v>3349668530045</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>534899</v>
+        <v>539811</v>
       </c>
       <c r="B21" s="1">
-        <v>3349667000013</v>
+        <v>3349668530069</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>539652</v>
+        <v>534899</v>
       </c>
       <c r="B22" s="1">
-        <v>3349668535675</v>
+        <v>3349667000013</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>540320</v>
+        <v>539652</v>
+      </c>
+      <c r="B23" s="1">
+        <v>3349668535675</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added logic to the final price with percentage and added them textboxes to the views.
</commit_message>
<xml_diff>
--- a/DBTester/wwwroot/UPC.xlsx
+++ b/DBTester/wwwroot/UPC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E338772C-4140-4CC9-9B89-48152F5AF0C9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9311E143-3025-4623-9A4E-1C97C482D4FF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -890,9 +890,6 @@
       <c r="A2">
         <v>540320</v>
       </c>
-      <c r="B2" s="1">
-        <v>3</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">

</xml_diff>